<commit_message>
Prueba de un archivo mas chico
</commit_message>
<xml_diff>
--- a/2015-08-19 ordenes de compra por comprador.xlsx
+++ b/2015-08-19 ordenes de compra por comprador.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mis documentos\Compradores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df21010b31a9c68c/Documentos/mis documentos/Compradores/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_A4E8E02A11E927BCD0EA11A6841C495BFE5784BD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7801FB9D-24A0-40B4-8A08-DB7D15A6C2C0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="DatosExternos_1" localSheetId="1" hidden="1">Hoja2!$A$1:$B$6</definedName>
+    <definedName name="DatosExternos_1" localSheetId="1" hidden="1">Hoja2!$A$1:$B$7</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,15 +29,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Consulta - Consulta1" description="Conexión a la consulta 'Consulta1' en el libro." type="5" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Consulta - Consulta1" description="Conexión a la consulta 'Consulta1' en el libro." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Consulta1;Extended Properties=&quot;&quot;" command="SELECT * FROM [Consulta1]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>UsuarioApertura</t>
   </si>
@@ -58,11 +59,14 @@
   <si>
     <t>nestor_niella</t>
   </si>
+  <si>
+    <t>ESTEBAN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -120,7 +124,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatosExternos_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DatosExternos_1" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="3">
     <queryTableFields count="2">
       <queryTableField id="1" name="UsuarioApertura" tableColumnId="5"/>
@@ -131,11 +135,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Consulta1" displayName="Consulta1" ref="A1:B6" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Consulta1" displayName="Consulta1" ref="A1:B7" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:B7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="5" uniqueName="5" name="UsuarioApertura" queryTableFieldId="1" dataDxfId="1"/>
-    <tableColumn id="6" uniqueName="6" name="cantidad" queryTableFieldId="2" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="UsuarioApertura" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="6" name="cantidad" queryTableFieldId="2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -403,7 +407,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -415,11 +419,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,6 +480,12 @@
         <v>326</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>